<commit_message>
Pequenas alterações na classificação
</commit_message>
<xml_diff>
--- a/Homem aranha.xlsx
+++ b/Homem aranha.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caior\OneDrive\Faculdade\2° PERÍODO\Ciência dos Dados\Projetos\CDados---Projeto-1-Arthur-e-Caio-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caior\OneDrive\Faculdade\2° PERÍODO\Ciência dos Dados\Projetos\Homem-Aranha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01CA60E-1861-4643-A93A-178FCB45F087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6384F8A6-23C0-4816-991F-08996E485316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2122,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B435"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>